<commit_message>
Refactor: Improve category count accuracy by loading mappings from an Excel file.  This removes hardcoded category logic and improves maintainability.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 99e232d0-2ccb-4f54-88fc-f8d7b049551e
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/b7e0e61d-cdc8-4899-899c-2d1b716c9906/a3e99da1-f93c-4537-b7d7-d1a4bf4733bd.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Categories Current.xlsx
+++ b/attached_assets/Categories Current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikki Lee\Desktop\TasteBuds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72FBB94-7C47-4E2C-815E-7377BEC2885D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D1C7C7-F8AB-4215-97F0-D5DCC6DF4765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50220" yWindow="1785" windowWidth="28635" windowHeight="12990" activeTab="1" xr2:uid="{167D6C32-A230-4D0D-B3FF-D3D329C28D80}"/>
+    <workbookView xWindow="-27150" yWindow="1650" windowWidth="17520" windowHeight="8985" activeTab="1" xr2:uid="{167D6C32-A230-4D0D-B3FF-D3D329C28D80}"/>
   </bookViews>
   <sheets>
     <sheet name="Items CSV Mapping" sheetId="7" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet2 (2)" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -233,19 +234,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,7 +568,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,7 +576,7 @@
       <c r="A1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C1" t="s">
@@ -587,577 +584,548 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="4">
         <v>81831</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>81990</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="4">
         <v>81990</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="4">
         <v>81991</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="4">
         <v>81991</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="4">
         <v>3074</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="4">
         <v>3001</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="4">
         <v>3009</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="4">
         <v>81828</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="4">
         <v>82151</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="4">
         <v>82149</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="4">
         <v>82147</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="4">
         <v>3033</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>3034</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="4">
         <v>3032</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="4">
         <v>81912</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="4">
         <v>3009</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="4">
         <v>3316</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="4">
         <v>3418</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="4">
         <v>81829</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="4">
         <v>2114</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="4">
         <v>2307</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="4">
         <v>3082</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="4">
         <v>3648</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="4">
         <v>2303</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="2"/>
-    </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="4">
         <v>2273</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="4">
         <v>2276</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="4">
         <v>2280</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="4">
         <v>81831</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="4">
         <v>81830</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="2"/>
-    </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="4">
         <v>2308</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="4">
         <v>3086</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="4">
         <v>3618</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="4">
         <v>2306</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="2"/>
-    </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="4">
         <v>2310</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="4">
         <v>3081</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="4">
         <v>3622</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="4">
         <v>2309</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1171,13 +1139,13 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1185,7 +1153,7 @@
       <c r="A1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C1" t="s">
@@ -1193,577 +1161,548 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="4">
         <v>81831</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>81990</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="4">
         <v>81990</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="4">
         <v>81991</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="4">
         <v>81991</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="4">
         <v>3074</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="4">
         <v>3001</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="4">
         <v>3009</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="4">
         <v>81828</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="4">
         <v>82151</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="4">
         <v>82149</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="4">
         <v>82147</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="4">
         <v>3033</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>3034</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="4">
         <v>3032</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="4">
         <v>81912</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="4">
         <v>3009</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="4">
         <v>3316</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="4">
         <v>3418</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="4">
         <v>81829</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="4">
         <v>2114</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="4">
         <v>2307</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="4">
         <v>3082</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="4">
         <v>3648</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="4">
         <v>2303</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="2"/>
-    </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="4">
         <v>2273</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="4">
         <v>2276</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="4">
         <v>2280</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="4">
         <v>81831</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="4">
         <v>81830</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="2"/>
-    </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="2"/>
     </row>
     <row r="52" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="4">
         <v>2308</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="4">
         <v>3086</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="4">
         <v>3618</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="4">
         <v>2306</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="2"/>
-    </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="7">
+      <c r="B59" s="4">
         <v>2310</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="4">
         <v>3081</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="7">
+      <c r="B61" s="4">
         <v>3622</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="7">
+      <c r="B62" s="4">
         <v>2309</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2358,6 +2297,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DateandTime xmlns="e52648fa-cf67-4b84-99d2-4f0b39f8a937" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e52648fa-cf67-4b84-99d2-4f0b39f8a937">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="82736d9a-06c9-4f65-8468-fb4b6b2e3d30" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003F5DAC6C2391F649896BAF83E1D4247D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="15850a5d6c1273f406857ada3dcc0ceb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e52648fa-cf67-4b84-99d2-4f0b39f8a937" xmlns:ns3="82736d9a-06c9-4f65-8468-fb4b6b2e3d30" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e0470506de140e512d646a59988a02b" ns2:_="" ns3:_="">
     <xsd:import namespace="e52648fa-cf67-4b84-99d2-4f0b39f8a937"/>
@@ -2598,28 +2558,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DateandTime xmlns="e52648fa-cf67-4b84-99d2-4f0b39f8a937" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e52648fa-cf67-4b84-99d2-4f0b39f8a937">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="82736d9a-06c9-4f65-8468-fb4b6b2e3d30" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E7DE27D-65D5-485A-9CDA-17782F7FA0BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58EBB967-6581-4110-9E88-23C46EB1667E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e52648fa-cf67-4b84-99d2-4f0b39f8a937"/>
+    <ds:schemaRef ds:uri="82736d9a-06c9-4f65-8468-fb4b6b2e3d30"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{763A13CE-C0A8-48FD-8462-0A683A98AE77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2636,23 +2594,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58EBB967-6581-4110-9E88-23C46EB1667E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e52648fa-cf67-4b84-99d2-4f0b39f8a937"/>
-    <ds:schemaRef ds:uri="82736d9a-06c9-4f65-8468-fb4b6b2e3d30"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E7DE27D-65D5-485A-9CDA-17782F7FA0BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>